<commit_message>
Add SQL script to removing redundant brand pairs
</commit_message>
<xml_diff>
--- a/Remove_Redundant_Pairs/Problem_Statement.xlsx
+++ b/Remove_Redundant_Pairs/Problem_Statement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thoufiq/THOUFIQ/techTFQ/YouTube/VIDEOS/30 SQL Interview Queries/Video_Q1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\30DaySQLQueryChallenge - techTFQ\Remove_Redundant_Pairs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DA700B1-3C94-6743-A136-70414E50288A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7355E001-D33C-42AB-928A-D0603FCA2DDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{D75DF9AA-5EB0-5C49-9364-B6DF4AF6325E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{D75DF9AA-5EB0-5C49-9364-B6DF4AF6325E}"/>
   </bookViews>
   <sheets>
     <sheet name="VIDEO_Q1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -168,7 +166,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>QUERY #1</t>
+      <t>#</t>
     </r>
     <r>
       <rPr>
@@ -533,15 +531,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -570,21 +559,30 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -921,132 +919,132 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBCD5299-05AF-E941-AC10-B7A2F7B9B1FB}">
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K17" sqref="K17"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2:H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="16384" width="10.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="19" x14ac:dyDescent="0.2">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.3">
+      <c r="A1" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-    </row>
-    <row r="2" spans="1:13" s="32" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="29"/>
-      <c r="B2" s="30" t="s">
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+    </row>
+    <row r="2" spans="1:13" s="27" customFormat="1" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="25"/>
+      <c r="B2" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-    </row>
-    <row r="3" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="31"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="31"/>
-      <c r="J3" s="31"/>
-      <c r="K3" s="31"/>
-      <c r="L3" s="31"/>
-    </row>
-    <row r="4" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="31"/>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
-      <c r="K4" s="31"/>
-      <c r="L4" s="31"/>
-    </row>
-    <row r="5" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="31"/>
-      <c r="B5" s="30"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="30"/>
-      <c r="I5" s="31"/>
-      <c r="J5" s="31"/>
-      <c r="K5" s="31"/>
-      <c r="L5" s="31"/>
-    </row>
-    <row r="6" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="31"/>
-      <c r="B6" s="30"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="31"/>
-      <c r="K6" s="31"/>
-      <c r="L6" s="31"/>
-    </row>
-    <row r="7" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="31"/>
-      <c r="B7" s="30"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
-    </row>
-    <row r="8" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="15" t="s">
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
+    </row>
+    <row r="3" spans="1:13" s="27" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="26"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+    </row>
+    <row r="4" spans="1:13" s="27" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="26"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
+    </row>
+    <row r="5" spans="1:13" s="27" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="26"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+    </row>
+    <row r="6" spans="1:13" s="27" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="26"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
+    </row>
+    <row r="7" spans="1:13" s="27" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="26"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="26"/>
+    </row>
+    <row r="8" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="9" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="17"/>
-    </row>
-    <row r="10" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="30"/>
+    </row>
+    <row r="10" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="2" t="s">
         <v>5</v>
       </c>
@@ -1069,151 +1067,151 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B11" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11" s="15">
         <v>2020</v>
       </c>
-      <c r="E11" s="18">
-        <v>1</v>
-      </c>
-      <c r="F11" s="18">
+      <c r="E11" s="15">
+        <v>1</v>
+      </c>
+      <c r="F11" s="15">
         <v>2</v>
       </c>
-      <c r="G11" s="18">
-        <v>1</v>
-      </c>
-      <c r="H11" s="19">
+      <c r="G11" s="15">
+        <v>1</v>
+      </c>
+      <c r="H11" s="16">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B12" s="11" t="s">
         <v>1</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D12" s="20">
+      <c r="D12" s="17">
         <v>2020</v>
       </c>
-      <c r="E12" s="20">
-        <v>1</v>
-      </c>
-      <c r="F12" s="20">
+      <c r="E12" s="17">
+        <v>1</v>
+      </c>
+      <c r="F12" s="17">
         <v>2</v>
       </c>
-      <c r="G12" s="20">
-        <v>1</v>
-      </c>
-      <c r="H12" s="21">
+      <c r="G12" s="17">
+        <v>1</v>
+      </c>
+      <c r="H12" s="18">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B13" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="22">
+      <c r="D13" s="19">
         <v>2021</v>
       </c>
-      <c r="E13" s="22">
-        <v>1</v>
-      </c>
-      <c r="F13" s="22">
+      <c r="E13" s="19">
+        <v>1</v>
+      </c>
+      <c r="F13" s="19">
         <v>2</v>
       </c>
-      <c r="G13" s="22">
+      <c r="G13" s="19">
         <v>5</v>
       </c>
-      <c r="H13" s="23">
+      <c r="H13" s="20">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B14" s="11" t="s">
         <v>1</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D14" s="20">
+      <c r="D14" s="17">
         <v>2021</v>
       </c>
-      <c r="E14" s="20">
+      <c r="E14" s="17">
         <v>5</v>
       </c>
-      <c r="F14" s="20">
+      <c r="F14" s="17">
         <v>3</v>
       </c>
-      <c r="G14" s="20">
-        <v>1</v>
-      </c>
-      <c r="H14" s="21">
+      <c r="G14" s="17">
+        <v>1</v>
+      </c>
+      <c r="H14" s="18">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B15" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C15" s="8"/>
-      <c r="D15" s="22">
+      <c r="D15" s="19">
         <v>2020</v>
       </c>
-      <c r="E15" s="22">
+      <c r="E15" s="19">
         <v>5</v>
       </c>
-      <c r="F15" s="22">
+      <c r="F15" s="19">
         <v>9</v>
       </c>
-      <c r="G15" s="22"/>
-      <c r="H15" s="23"/>
-    </row>
-    <row r="16" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G15" s="19"/>
+      <c r="H15" s="20"/>
+    </row>
+    <row r="16" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="13" t="s">
         <v>3</v>
       </c>
       <c r="C16" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D16" s="24">
+      <c r="D16" s="21">
         <v>2020</v>
       </c>
-      <c r="E16" s="24">
+      <c r="E16" s="21">
         <v>5</v>
       </c>
-      <c r="F16" s="24">
+      <c r="F16" s="21">
         <v>9</v>
       </c>
-      <c r="G16" s="24">
+      <c r="G16" s="21">
         <v>6</v>
       </c>
-      <c r="H16" s="25">
+      <c r="H16" s="22">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="15" t="s">
+    <row r="17" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="18" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="17"/>
-    </row>
-    <row r="19" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="30"/>
+    </row>
+    <row r="19" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="2" t="s">
         <v>5</v>
       </c>
@@ -1236,114 +1234,114 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B20" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D20" s="18">
+      <c r="D20" s="15">
         <v>2020</v>
       </c>
-      <c r="E20" s="18">
-        <v>1</v>
-      </c>
-      <c r="F20" s="18">
+      <c r="E20" s="15">
+        <v>1</v>
+      </c>
+      <c r="F20" s="15">
         <v>2</v>
       </c>
-      <c r="G20" s="18">
-        <v>1</v>
-      </c>
-      <c r="H20" s="19">
+      <c r="G20" s="15">
+        <v>1</v>
+      </c>
+      <c r="H20" s="16">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B21" s="11" t="s">
         <v>0</v>
       </c>
       <c r="C21" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D21" s="20">
+      <c r="D21" s="17">
         <v>2021</v>
       </c>
-      <c r="E21" s="20">
-        <v>1</v>
-      </c>
-      <c r="F21" s="20">
+      <c r="E21" s="17">
+        <v>1</v>
+      </c>
+      <c r="F21" s="17">
         <v>2</v>
       </c>
-      <c r="G21" s="20">
+      <c r="G21" s="17">
         <v>5</v>
       </c>
-      <c r="H21" s="21">
+      <c r="H21" s="18">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B22" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D22" s="22">
+      <c r="D22" s="19">
         <v>2021</v>
       </c>
-      <c r="E22" s="22">
+      <c r="E22" s="19">
         <v>5</v>
       </c>
-      <c r="F22" s="22">
+      <c r="F22" s="19">
         <v>3</v>
       </c>
-      <c r="G22" s="22">
-        <v>1</v>
-      </c>
-      <c r="H22" s="23">
+      <c r="G22" s="19">
+        <v>1</v>
+      </c>
+      <c r="H22" s="20">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B23" s="11" t="s">
         <v>3</v>
       </c>
       <c r="C23" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D23" s="20">
+      <c r="D23" s="17">
         <v>2020</v>
       </c>
-      <c r="E23" s="20">
+      <c r="E23" s="17">
         <v>5</v>
       </c>
-      <c r="F23" s="20">
+      <c r="F23" s="17">
         <v>9</v>
       </c>
-      <c r="G23" s="20">
+      <c r="G23" s="17">
         <v>6</v>
       </c>
-      <c r="H23" s="21">
+      <c r="H23" s="18">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="9" t="s">
         <v>2</v>
       </c>
       <c r="C24" s="10"/>
-      <c r="D24" s="26">
+      <c r="D24" s="23">
         <v>2020</v>
       </c>
-      <c r="E24" s="26">
+      <c r="E24" s="23">
         <v>5</v>
       </c>
-      <c r="F24" s="26">
+      <c r="F24" s="23">
         <v>9</v>
       </c>
-      <c r="G24" s="26"/>
-      <c r="H24" s="27"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>